<commit_message>
Add examples with ubday constrains
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/33-assign-423-no-pbsum/33-assign-423-no-pbsum.xlsx
+++ b/ampl-data-input-excel/33-assign-423-no-pbsum/33-assign-423-no-pbsum.xlsx
@@ -1329,7 +1329,7 @@
     <t xml:space="preserve">highs</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes</t>
+    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">Width</t>
@@ -2469,7 +2469,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>